<commit_message>
?? ????? ?? ???????? ???? ???? ????. ?????????????? ???? ???????? ?? ???????? :)
</commit_message>
<xml_diff>
--- a/src/tests/test_data/linux/test-simple.xlsx
+++ b/src/tests/test_data/linux/test-simple.xlsx
@@ -49,6 +49,19 @@
         </r>
       </text>
     </comment>
+    <comment authorId="0" ref="D7">
+      <text>
+        <r>
+          <rPr>
+            <rFont val="Arial"/>
+            <charset val="1"/>
+            <family val="2"/>
+            <sz val="10"/>
+          </rPr>
+          <t xml:space="preserve">-A1</t>
+        </r>
+      </text>
+    </comment>
     <comment authorId="0" ref="F7">
       <text>
         <r>
@@ -59,19 +72,6 @@
             <sz val="10"/>
           </rPr>
           <t xml:space="preserve">-GOR</t>
-        </r>
-      </text>
-    </comment>
-    <comment authorId="0" ref="E8">
-      <text>
-        <r>
-          <rPr>
-            <rFont val="Arial"/>
-            <charset val="1"/>
-            <family val="2"/>
-            <sz val="10"/>
-          </rPr>
-          <t xml:space="preserve">-A1</t>
         </r>
       </text>
     </comment>
@@ -409,7 +409,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
   <si>
     <t>Добро пожаловать #user#</t>
   </si>
@@ -417,37 +417,40 @@
     <t>Сегодня: #date_now#</t>
   </si>
   <si>
+    <t>ФИО Участок</t>
+  </si>
+  <si>
     <t>#col#</t>
   </si>
   <si>
     <t>Номер</t>
   </si>
   <si>
+    <t>Просто тупо текст</t>
+  </si>
+  <si>
+    <t>Т</t>
+  </si>
+  <si>
+    <t>#nbr#</t>
+  </si>
+  <si>
+    <t>#fio#</t>
+  </si>
+  <si>
+    <t>#sector#</t>
+  </si>
+  <si>
+    <t>#g#</t>
+  </si>
+  <si>
+    <t>Подпись уполномоченного сотрудника: #user#</t>
+  </si>
+  <si>
     <t>ФИО</t>
   </si>
   <si>
     <t>Участок</t>
-  </si>
-  <si>
-    <t>Просто тупо текст</t>
-  </si>
-  <si>
-    <t>Т</t>
-  </si>
-  <si>
-    <t>#nbr#</t>
-  </si>
-  <si>
-    <t>#fio#</t>
-  </si>
-  <si>
-    <t>#sector#</t>
-  </si>
-  <si>
-    <t>#g#</t>
-  </si>
-  <si>
-    <t>Подпись уполномоченного сотрудника: #user#</t>
   </si>
 </sst>
 </file>
@@ -551,9 +554,12 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
@@ -641,16 +647,16 @@
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
-      <selection activeCell="C18" activeCellId="0" pane="topLeft" sqref="C18"/>
+      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
       <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7921568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="48.5" outlineLevel="0" r="5">
@@ -666,46 +672,46 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="I8" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="F10" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="n">
@@ -713,8 +719,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C5:E5"/>
+    <mergeCell ref="D7:E8"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -741,7 +748,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
@@ -757,36 +764,36 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -818,7 +825,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
@@ -834,36 +841,36 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
-      <c r="D9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="E9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="D11" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -895,7 +902,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.68235294117647"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -916,36 +923,36 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
-      <c r="F11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="G11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="E12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="F13" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="14">
@@ -954,14 +961,14 @@
       <c r="H14" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="17">
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="18">
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
?????????? ??????, ????????? ? ???, ??? ??? ????????? ? ????? ?????? ?????? ???? ????????????
</commit_message>
<xml_diff>
--- a/src/tests/test_data/linux/test-simple.xlsx
+++ b/src/tests/test_data/linux/test-simple.xlsx
@@ -409,7 +409,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
   <si>
     <t>Добро пожаловать #user#</t>
   </si>
@@ -435,22 +435,29 @@
     <t>#nbr#</t>
   </si>
   <si>
+    <t>#fio# ага  #nbr#</t>
+  </si>
+  <si>
+    <t>#sector# фыв 
+#nbr#</t>
+  </si>
+  <si>
+    <t>#g#</t>
+  </si>
+  <si>
+    <t>Подпись уполномоченного сотрудника: #user#</t>
+  </si>
+  <si>
+    <t>ФИО</t>
+  </si>
+  <si>
+    <t>Участок</t>
+  </si>
+  <si>
     <t>#fio#</t>
   </si>
   <si>
     <t>#sector#</t>
-  </si>
-  <si>
-    <t>#g#</t>
-  </si>
-  <si>
-    <t>Подпись уполномоченного сотрудника: #user#</t>
-  </si>
-  <si>
-    <t>ФИО</t>
-  </si>
-  <si>
-    <t>Участок</t>
   </si>
 </sst>
 </file>
@@ -554,7 +561,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -564,6 +571,9 @@
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
   </cellXfs>
@@ -647,16 +657,16 @@
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
-      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
+      <selection activeCell="F14" activeCellId="0" pane="topLeft" sqref="F14"/>
       <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.72941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7921568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.72941176470588"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.81960784313726"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="48.5" outlineLevel="0" r="5">
@@ -690,7 +700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="9">
       <c r="B9" s="0" t="s">
         <v>6</v>
       </c>
@@ -700,10 +710,10 @@
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -711,7 +721,7 @@
       <c r="C10" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="n">
@@ -748,7 +758,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81960784313726"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
@@ -785,10 +795,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
@@ -825,7 +835,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81960784313726"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
@@ -862,10 +872,10 @@
         <v>7</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
@@ -902,7 +912,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.77254901960784"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -944,10 +954,10 @@
         <v>7</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">

</xml_diff>

<commit_message>
? ???????????? ??????? ?????????? ?????? ?????????? ??????, ? ????? ? ??? ????????? ??????????? ?????? ??????????, ? ??????? ???????????? ????????? ??????? ????????? ???????????.
</commit_message>
<xml_diff>
--- a/src/tests/test_data/linux/test-simple.xlsx
+++ b/src/tests/test_data/linux/test-simple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="175" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="276" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,20 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="D7">
+    <comment authorId="0" ref="F7">
+      <text>
+        <r>
+          <rPr>
+            <rFont val="Arial"/>
+            <charset val="1"/>
+            <family val="2"/>
+            <sz val="10"/>
+          </rPr>
+          <t xml:space="preserve">-GOR</t>
+        </r>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E8">
       <text>
         <r>
           <rPr>
@@ -59,19 +72,6 @@
             <sz val="10"/>
           </rPr>
           <t xml:space="preserve">-A1</t>
-        </r>
-      </text>
-    </comment>
-    <comment authorId="0" ref="F7">
-      <text>
-        <r>
-          <rPr>
-            <rFont val="Arial"/>
-            <charset val="1"/>
-            <family val="2"/>
-            <sz val="10"/>
-          </rPr>
-          <t xml:space="preserve">-GOR</t>
         </r>
       </text>
     </comment>
@@ -409,7 +409,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
   <si>
     <t>Добро пожаловать #user#</t>
   </si>
@@ -417,15 +417,18 @@
     <t>Сегодня: #date_now#</t>
   </si>
   <si>
-    <t>ФИО Участок</t>
-  </si>
-  <si>
     <t>#col#</t>
   </si>
   <si>
     <t>Номер</t>
   </si>
   <si>
+    <t>ФИО</t>
+  </si>
+  <si>
+    <t>Участок</t>
+  </si>
+  <si>
     <t>Просто тупо текст</t>
   </si>
   <si>
@@ -435,41 +438,27 @@
     <t>#nbr#</t>
   </si>
   <si>
-    <t>#fio# ага  #nbr#</t>
-  </si>
-  <si>
-    <t>#sector# фыв 
-#nbr#</t>
+    <t>#fio#</t>
+  </si>
+  <si>
+    <t>#sector#</t>
   </si>
   <si>
     <t>#g#</t>
   </si>
   <si>
     <t>Подпись уполномоченного сотрудника: #user#</t>
-  </si>
-  <si>
-    <t>ФИО</t>
-  </si>
-  <si>
-    <t>Участок</t>
-  </si>
-  <si>
-    <t>#fio#</t>
-  </si>
-  <si>
-    <t>#sector#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="0" numFmtId="165"/>
-    <numFmt formatCode="#,#00" numFmtId="166"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -498,27 +487,13 @@
       <b val="true"/>
       <sz val="10"/>
     </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="10"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFF66"/>
-        <bgColor rgb="00FFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -562,21 +537,13 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -586,66 +553,6 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF66"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -658,16 +565,16 @@
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
-      <selection activeCell="G9" activeCellId="0" pane="topLeft" sqref="G9"/>
+      <selection activeCell="F14" activeCellId="0" pane="topLeft" sqref="F14"/>
       <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.86274509803922"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1019607843137"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.86274509803922"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2823529411765"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.9647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.078431372549"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9647058823529"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.9647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="48.5" outlineLevel="0" r="5">
@@ -683,46 +590,45 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
+      <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="I8" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="B9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="7"/>
+        <v>12</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="n">
@@ -730,9 +636,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="C5:E5"/>
-    <mergeCell ref="D7:E8"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -759,7 +664,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
@@ -775,36 +680,36 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>13</v>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="B9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -836,7 +741,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
@@ -852,36 +757,36 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>13</v>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>15</v>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="D11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -913,7 +818,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9019607843137"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -934,36 +839,36 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>13</v>
+      <c r="H11" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="E12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>15</v>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="F13" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="14">
@@ -972,14 +877,14 @@
       <c r="H14" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="17">
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="18">
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
???????? ???????? ????????? ????? + ????????? ???? ? ???
</commit_message>
<xml_diff>
--- a/src/tests/test_data/linux/test-simple.xlsx
+++ b/src/tests/test_data/linux/test-simple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="276" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="3" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
@@ -409,54 +409,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
   <si>
     <t>Добро пожаловать #user#</t>
   </si>
   <si>
+    <t>Сегодня: #%DATE_NOW%#</t>
+  </si>
+  <si>
+    <t>#%test_tag%#</t>
+  </si>
+  <si>
+    <t>#%DATE_NOW%#</t>
+  </si>
+  <si>
+    <t>#col#</t>
+  </si>
+  <si>
+    <t>Номер</t>
+  </si>
+  <si>
+    <t>ФИО</t>
+  </si>
+  <si>
+    <t>Участок</t>
+  </si>
+  <si>
+    <t>Просто тупо текст</t>
+  </si>
+  <si>
+    <t>Т</t>
+  </si>
+  <si>
+    <t>#nbr#</t>
+  </si>
+  <si>
+    <t>#fio#</t>
+  </si>
+  <si>
+    <t>#sector#</t>
+  </si>
+  <si>
+    <t>#g#</t>
+  </si>
+  <si>
+    <t>Подпись уполномоченного сотрудника: #user#</t>
+  </si>
+  <si>
     <t>Сегодня: #date_now#</t>
-  </si>
-  <si>
-    <t>#col#</t>
-  </si>
-  <si>
-    <t>Номер</t>
-  </si>
-  <si>
-    <t>ФИО</t>
-  </si>
-  <si>
-    <t>Участок</t>
-  </si>
-  <si>
-    <t>Просто тупо текст</t>
-  </si>
-  <si>
-    <t>Т</t>
-  </si>
-  <si>
-    <t>#nbr#</t>
-  </si>
-  <si>
-    <t>#fio#</t>
-  </si>
-  <si>
-    <t>#sector#</t>
-  </si>
-  <si>
-    <t>#g#</t>
-  </si>
-  <si>
-    <t>Подпись уполномоченного сотрудника: #user#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0" numFmtId="165"/>
+    <numFmt formatCode="DD/MM/YYYY\ HH:MM:SS" numFmtId="165"/>
+    <numFmt formatCode="0" numFmtId="166"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -537,13 +547,14 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -565,16 +576,16 @@
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
-      <selection activeCell="F14" activeCellId="0" pane="topLeft" sqref="F14"/>
+      <selection activeCell="D6" activeCellId="0" pane="topLeft" sqref="D6"/>
       <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.9647058823529"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.078431372549"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9647058823529"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.9647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.95294117647059"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.1490196078431"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.9803921568627"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.95294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="48.5" outlineLevel="0" r="5">
@@ -588,46 +599,52 @@
       <c r="C6" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="D6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="F7" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I8" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="B9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="F9" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
@@ -664,7 +681,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.95294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
@@ -676,40 +693,40 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="H7" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -741,7 +758,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.95294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
@@ -753,40 +770,40 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="D7" s="0" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
-      <c r="D9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="J9" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="D11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -818,7 +835,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.90980392156863"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -835,40 +852,40 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="F9" s="0" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
-      <c r="F11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="L11" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="E12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="F13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="14">
@@ -877,14 +894,14 @@
       <c r="H14" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="17">
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="18">
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>